<commit_message>
Update Q&A data set...... :sob:
Add available questions list and available questions fields.
작업하다가 보니 저 행정학과로 전직한 느낌이에요...
</commit_message>
<xml_diff>
--- a/톡톡120질문답변_upload_kim.xlsx
+++ b/톡톡120질문답변_upload_kim.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="108">
   <si>
     <t>영유아 건강검진</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -572,6 +572,83 @@
   <si>
     <t>▣ 임산부, 영유아 등록관리 주의사항
     보건복지부 임신.출산.육아정보 포털사이트 : 아가사랑(http://www.agasarang.org)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>질문 가능한 목록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>질문 가능한 분야</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>▣ 서아키 챗봇이 대답 가능한 질문 분야
+▷ 임신, 출산
+▷ 육아
+▷ 질병, 치료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>▣ 서아키 챗봇이 대답 가능한 질문 목록
+▷ 임신, 출산
+＊ 임산부 등록
+＊ 산전검사 문의
+＊ 산전검사 예약 및 이력 확인
+＊ 산후조리원
+＊ 산모지원 기타
+＊ 난임부부
+＊ 양천구 임산부 엽산제 지급 지원
+＊ 양천구 임산부 철분제 지급 지원
+＊ 양천구 임산부 토요 진료 지원
+＊ 임산부 철분제 공급 신청방법
+＊ 임산부 철분제 공급 구비서류
+＊ 임산부 철분제 공급 접수처
+＊ 임산부, 영유아 등록관리 접수처
+＊ 임산부, 영유아 등록관리 신청방법
+＊ 임산부, 영유아 등록관리 구비서류
+＊ 임산부 산전관리 목록
+＊ 임산부 산후관리 목록
+＊ 임산부 영유아 관리
+＊ 임산부 신고 ㆍ등록관리
+＊ 고운맘 카드를 통한 임신.출산 진료비 지원 사업 소개
+＊ 임신 중기의 모자의 건강 및 태내 성장 증진을 위한 철분제 지원
+＊ 임산부 등에 대한 산ㆍ전후 우울증 진단 및 사후관리 안내, 교육강화, 상담 등 우울증 예방,관리 강화
+＊ 임부에 대한 산전관리의 중요성 및 홍보를 통해 안전 분만 또는 자연분만 적극 유도
+＊ 고위험 임산부 특별관리
+＊ 임산부, 영유아 등록관리 주의사항
+＊ 고위험 임산부 의료비 지원 대상자
+▷ 육아
+＊ 영유아 건강검진
+＊ 영유아 발달지원
+＊ 영유아 예방접종
+＊ 서울아기 건강 첫걸음 사업
+＊ 신생아 지원
+＊ 어린이집 보육료 지원
+＊ 어린이집 입소대기
+＊ 보육포털서비스
+＊ 어린이집 보육료 지원
+▷ 질병, 치료
+＊ 병원 정보 확인하기
+＊ A형간염
+＊ B형간염
+＊ 감염병 일반 문의
+＊ 결핵
+＊ 결핵 관리
+＊ 난청
+＊ 심뇌혈관질환
+＊ 난청
+＊ 대사증후군
+＊ 예방접종 대상
+＊ 예방접종 횟수
+＊ 예방접종 장소
+＊ 2019-2020절기 인플루엔자 국가예방접종 지원사업 대상자
+＊ 2019-2020절기 인플루엔자 국가예방접종 지원사업 기간
+＊ 2019-2020절기 인플루엔자 국가예방접종 지원사업 실시기관
+＊ 2019-2020절기 인플루엔자 국가예방접종 지원사업 비용
+▷ 챗봇 도움말
+＊ 질문 가능한 분야
+＊ 질문 가능한 목록</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1049,10 +1126,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M59"/>
+  <dimension ref="A1:M62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I58" sqref="I58:I59"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1067,7 +1144,7 @@
     <col min="14" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="143.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="133.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -1081,62 +1158,50 @@
         <v>23</v>
       </c>
       <c r="H1" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="330" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I3" s="9" t="s">
         <v>41</v>
-      </c>
-      <c r="L1" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="M1" s="10">
-        <v>43745</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="247.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="L2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="M2" s="10">
-        <v>43745</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="214.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>43</v>
       </c>
       <c r="L3" s="1" t="b">
         <v>1</v>
@@ -1145,7 +1210,7 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="247.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1159,10 +1224,10 @@
         <v>23</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L4" s="1" t="b">
         <v>1</v>
@@ -1171,7 +1236,7 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="198" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="214.5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -1185,10 +1250,10 @@
         <v>23</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L5" s="1" t="b">
         <v>1</v>
@@ -1197,7 +1262,7 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="264" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -1211,10 +1276,10 @@
         <v>23</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L6" s="1" t="b">
         <v>1</v>
@@ -1237,10 +1302,10 @@
         <v>23</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L7" s="1" t="b">
         <v>1</v>
@@ -1249,7 +1314,7 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="297" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="264" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1263,10 +1328,10 @@
         <v>23</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L8" s="1" t="b">
         <v>1</v>
@@ -1275,7 +1340,7 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="181.5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -1289,10 +1354,10 @@
         <v>23</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>49</v>
+        <v>6</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="L9" s="1" t="b">
         <v>1</v>
@@ -1301,7 +1366,7 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="330" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="297" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -1315,10 +1380,10 @@
         <v>23</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L10" s="1" t="b">
         <v>1</v>
@@ -1327,7 +1392,7 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="198" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -1341,10 +1406,10 @@
         <v>23</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>51</v>
+        <v>8</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="L11" s="1" t="b">
         <v>1</v>
@@ -1353,7 +1418,7 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="330" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -1367,10 +1432,10 @@
         <v>23</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="L12" s="1" t="b">
         <v>1</v>
@@ -1393,10 +1458,10 @@
         <v>23</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L13" s="1" t="b">
         <v>1</v>
@@ -1405,7 +1470,7 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="198" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1419,10 +1484,10 @@
         <v>23</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>53</v>
+        <v>11</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="L14" s="1" t="b">
         <v>1</v>
@@ -1431,7 +1496,7 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="363" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="198" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
@@ -1445,10 +1510,10 @@
         <v>23</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="L15" s="1" t="b">
         <v>1</v>
@@ -1457,7 +1522,7 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="297" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="198" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
@@ -1471,10 +1536,10 @@
         <v>23</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="L16" s="1" t="b">
         <v>1</v>
@@ -1483,7 +1548,7 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="247.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="363" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -1497,10 +1562,10 @@
         <v>23</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="L17" s="1" t="b">
         <v>1</v>
@@ -1509,7 +1574,7 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="330" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="297" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -1523,10 +1588,10 @@
         <v>23</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="L18" s="1" t="b">
         <v>1</v>
@@ -1549,10 +1614,10 @@
         <v>23</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L19" s="1" t="b">
         <v>1</v>
@@ -1574,71 +1639,83 @@
       <c r="D20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" s="8" t="s">
         <v>18</v>
       </c>
       <c r="I20" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="L20" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M20" s="10">
+        <v>43745</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="280.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="L21" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="M21" s="10">
+        <v>43745</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="330" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="247.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H21" s="1" t="s">
+    <row r="23" spans="1:13" ht="247.5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I21" s="9" t="s">
+      <c r="I23" s="9" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="231" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
@@ -1655,113 +1732,113 @@
         <v>23</v>
       </c>
       <c r="H24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="231" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="I26" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H25" s="3" t="s">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="I27" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H26" s="1" t="s">
+    <row r="28" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I26" s="5" t="s">
+      <c r="I28" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H27" s="1" t="s">
+    <row r="29" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I27" s="6" t="s">
+      <c r="I29" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="346.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="297" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I29" s="9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" ht="346.5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>20</v>
       </c>
@@ -1775,13 +1852,13 @@
         <v>28</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I30" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="346.5" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="297" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>20</v>
       </c>
@@ -1795,53 +1872,53 @@
         <v>28</v>
       </c>
       <c r="H31" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="346.5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I31" s="7" t="s">
+      <c r="I33" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="280.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="409.5" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I33" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="409.5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="280.5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>20</v>
       </c>
@@ -1855,13 +1932,13 @@
         <v>63</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="148.5" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>20</v>
       </c>
@@ -1875,10 +1952,10 @@
         <v>63</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="237.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1895,10 +1972,10 @@
         <v>63</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1915,13 +1992,13 @@
         <v>63</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="148.5" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="313.5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>20</v>
       </c>
@@ -1935,13 +2012,13 @@
         <v>63</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="247.5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>20</v>
       </c>
@@ -1955,13 +2032,13 @@
         <v>63</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>20</v>
       </c>
@@ -1975,13 +2052,13 @@
         <v>63</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>20</v>
       </c>
@@ -1995,13 +2072,13 @@
         <v>63</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="409.5" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>20</v>
       </c>
@@ -2015,13 +2092,13 @@
         <v>63</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="216" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>20</v>
       </c>
@@ -2035,13 +2112,13 @@
         <v>63</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="I43" s="12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="330" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>20</v>
       </c>
@@ -2055,13 +2132,13 @@
         <v>63</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="I44" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="409.5" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="216" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>20</v>
       </c>
@@ -2075,13 +2152,13 @@
         <v>63</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I45" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="409.5" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="I45" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="330" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>20</v>
       </c>
@@ -2095,10 +2172,10 @@
         <v>63</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="409.5" x14ac:dyDescent="0.3">
@@ -2115,13 +2192,13 @@
         <v>63</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="396" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>20</v>
       </c>
@@ -2135,13 +2212,13 @@
         <v>63</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="214.5" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>20</v>
       </c>
@@ -2155,13 +2232,13 @@
         <v>63</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="409.5" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="396" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>20</v>
       </c>
@@ -2175,13 +2252,13 @@
         <v>63</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I50" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="165" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="214.5" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>20</v>
       </c>
@@ -2195,14 +2272,57 @@
         <v>63</v>
       </c>
       <c r="H51" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I51" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I52" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="165" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H53" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="I51" s="7" t="s">
+      <c r="I53" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I59" s="11"/>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I54" s="7"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I62" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>